<commit_message>
algoritmo 2 e escrever para ficheiro agora com decisão
</commit_message>
<xml_diff>
--- a/auxiliares/txt criado explicado.xlsx
+++ b/auxiliares/txt criado explicado.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="EVENTOS" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="258">
   <si>
     <t>EVENTOS</t>
   </si>
@@ -883,6 +883,15 @@
   </si>
   <si>
     <t>Amigos do primo do coiso;</t>
+  </si>
+  <si>
+    <t>aqui não deviam ser apenas sem candidaturas</t>
+  </si>
+  <si>
+    <t>e tenham candidaturas atribuidas</t>
+  </si>
+  <si>
+    <t>e não tenham decisao</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1056,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1057,11 +1071,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1381,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1432,6 +1441,9 @@
       <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -1448,6 +1460,12 @@
       </c>
       <c r="E5" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -1523,13 +1541,13 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1555,40 +1573,40 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1601,26 +1619,26 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -2073,7 +2091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2097,7 +2115,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -2112,7 +2130,7 @@
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
+      <c r="A3" s="20"/>
       <c r="B3" s="2" t="s">
         <v>82</v>
       </c>
@@ -2125,7 +2143,7 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>82</v>
       </c>
@@ -2154,7 +2172,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
@@ -2183,7 +2201,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2" t="s">
         <v>82</v>
       </c>
@@ -2212,7 +2230,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="7" t="s">
         <v>83</v>
       </c>
@@ -2243,7 +2261,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2" t="s">
         <v>83</v>
       </c>
@@ -2276,7 +2294,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
@@ -2289,7 +2307,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="2" t="s">
         <v>83</v>
       </c>
@@ -2302,7 +2320,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="2" t="s">
         <v>83</v>
       </c>
@@ -2315,7 +2333,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="7" t="s">
         <v>84</v>
       </c>
@@ -2331,7 +2349,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="10" t="s">
         <v>84</v>
       </c>
@@ -2365,7 +2383,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="2" t="s">
         <v>84</v>
       </c>
@@ -2397,7 +2415,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="2" t="s">
         <v>84</v>
       </c>
@@ -2411,7 +2429,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="2" t="s">
         <v>84</v>
       </c>
@@ -2422,7 +2440,7 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="7" t="s">
         <v>85</v>
       </c>
@@ -2435,7 +2453,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="2" t="s">
         <v>85</v>
       </c>
@@ -2451,7 +2469,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="2" t="s">
         <v>85</v>
       </c>
@@ -2462,7 +2480,7 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="2" t="s">
         <v>85</v>
       </c>
@@ -2473,7 +2491,7 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="2" t="s">
         <v>85</v>
       </c>
@@ -2487,7 +2505,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -2505,7 +2523,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="2" t="s">
         <v>86</v>
       </c>
@@ -2518,7 +2536,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="2" t="s">
         <v>86</v>
       </c>
@@ -2532,7 +2550,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="2" t="s">
         <v>86</v>
       </c>
@@ -2543,7 +2561,7 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="2" t="s">
         <v>86</v>
       </c>
@@ -2554,7 +2572,7 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="8" t="s">
         <v>87</v>
       </c>
@@ -2570,7 +2588,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
@@ -2586,7 +2604,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="2" t="s">
         <v>87</v>
       </c>
@@ -2597,7 +2615,7 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="2" t="s">
         <v>87</v>
       </c>
@@ -2608,7 +2626,7 @@
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="2" t="s">
         <v>87</v>
       </c>
@@ -2622,7 +2640,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="8" t="s">
         <v>88</v>
       </c>
@@ -2635,7 +2653,7 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="15"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="2" t="s">
         <v>88</v>
       </c>
@@ -2648,7 +2666,7 @@
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="2" t="s">
         <v>88</v>
       </c>
@@ -2662,7 +2680,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="2" t="s">
         <v>88</v>
       </c>
@@ -2676,7 +2694,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="2" t="s">
         <v>88</v>
       </c>
@@ -2690,7 +2708,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="8" t="s">
         <v>89</v>
       </c>
@@ -2703,7 +2721,7 @@
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="2" t="s">
         <v>89</v>
       </c>
@@ -2716,7 +2734,7 @@
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="2" t="s">
         <v>89</v>
       </c>
@@ -2730,7 +2748,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="2" t="s">
         <v>89</v>
       </c>
@@ -2744,7 +2762,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="15"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="2" t="s">
         <v>89</v>
       </c>
@@ -2758,7 +2776,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -2776,7 +2794,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="16"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="2" t="s">
         <v>90</v>
       </c>
@@ -2792,7 +2810,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="16"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="2" t="s">
         <v>90</v>
       </c>
@@ -2806,7 +2824,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="16"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="2" t="s">
         <v>90</v>
       </c>
@@ -2817,7 +2835,7 @@
       <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="16"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2828,7 +2846,7 @@
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="16"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="9" t="s">
         <v>91</v>
       </c>
@@ -2841,7 +2859,7 @@
       <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="16"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="2" t="s">
         <v>91</v>
       </c>
@@ -2854,7 +2872,7 @@
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="16"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="2" t="s">
         <v>91</v>
       </c>
@@ -2865,7 +2883,7 @@
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="16"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="2" t="s">
         <v>91</v>
       </c>
@@ -2876,7 +2894,7 @@
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="16"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="2" t="s">
         <v>91</v>
       </c>
@@ -2887,7 +2905,7 @@
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="16"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="9" t="s">
         <v>92</v>
       </c>
@@ -2900,7 +2918,7 @@
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="16"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="2" t="s">
         <v>92</v>
       </c>
@@ -2913,7 +2931,7 @@
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="16"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="2" t="s">
         <v>92</v>
       </c>
@@ -2924,7 +2942,7 @@
       <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="16"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="2" t="s">
         <v>92</v>
       </c>
@@ -2935,7 +2953,7 @@
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="16"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="2" t="s">
         <v>92</v>
       </c>
@@ -2946,7 +2964,7 @@
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="16"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="9" t="s">
         <v>93</v>
       </c>
@@ -2959,7 +2977,7 @@
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="16"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="2" t="s">
         <v>93</v>
       </c>
@@ -2972,7 +2990,7 @@
       <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="16"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="2" t="s">
         <v>93</v>
       </c>
@@ -2981,7 +2999,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="16"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="2" t="s">
         <v>93</v>
       </c>
@@ -2990,7 +3008,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="16"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="2" t="s">
         <v>93</v>
       </c>
@@ -3056,13 +3074,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2"/>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D68" s="20" t="s">
+      <c r="D68" s="15" t="s">
         <v>99</v>
       </c>
       <c r="E68" s="2"/>
@@ -3070,13 +3088,13 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2"/>
-      <c r="B69" s="19" t="s">
+      <c r="B69" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="15" t="s">
         <v>100</v>
       </c>
       <c r="E69" s="2"/>
@@ -3084,26 +3102,26 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2"/>
-      <c r="B70" s="19" t="s">
+      <c r="B70" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="C70" s="20" t="s">
+      <c r="C70" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="D70" s="20" t="s">
+      <c r="D70" s="15" t="s">
         <v>99</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D71" s="20" t="s">
+      <c r="D71" s="15" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3141,7 +3159,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -3155,7 +3173,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>82</v>
       </c>
@@ -3167,7 +3185,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
@@ -3179,7 +3197,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2" t="s">
         <v>82</v>
       </c>
@@ -3191,7 +3209,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="2" t="s">
         <v>82</v>
       </c>
@@ -3203,7 +3221,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="7" t="s">
         <v>83</v>
       </c>
@@ -3215,7 +3233,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="2" t="s">
         <v>83</v>
       </c>
@@ -3227,7 +3245,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="2" t="s">
         <v>83</v>
       </c>
@@ -3239,7 +3257,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
         <v>84</v>
       </c>
@@ -3251,7 +3269,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="10" t="s">
         <v>84</v>
       </c>
@@ -3263,7 +3281,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="2" t="s">
         <v>84</v>
       </c>
@@ -3275,7 +3293,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="2" t="s">
         <v>84</v>
       </c>
@@ -3287,7 +3305,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="2" t="s">
         <v>84</v>
       </c>
@@ -3299,7 +3317,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="2" t="s">
         <v>84</v>
       </c>
@@ -3311,7 +3329,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="7" t="s">
         <v>85</v>
       </c>
@@ -3323,7 +3341,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="2" t="s">
         <v>85</v>
       </c>
@@ -3332,7 +3350,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="2" t="s">
         <v>85</v>
       </c>
@@ -3341,7 +3359,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="2" t="s">
         <v>85</v>
       </c>
@@ -3350,7 +3368,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -3361,7 +3379,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="2" t="s">
         <v>86</v>
       </c>
@@ -3370,7 +3388,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="2" t="s">
         <v>86</v>
       </c>
@@ -3379,7 +3397,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="2" t="s">
         <v>86</v>
       </c>
@@ -3388,7 +3406,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="2" t="s">
         <v>86</v>
       </c>
@@ -3397,7 +3415,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="8" t="s">
         <v>87</v>
       </c>
@@ -3406,7 +3424,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="2" t="s">
         <v>87</v>
       </c>
@@ -3415,7 +3433,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
@@ -3424,7 +3442,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="8" t="s">
         <v>88</v>
       </c>
@@ -3433,7 +3451,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="2" t="s">
         <v>88</v>
       </c>
@@ -3442,7 +3460,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="2" t="s">
         <v>88</v>
       </c>
@@ -3451,7 +3469,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="2" t="s">
         <v>88</v>
       </c>
@@ -3460,7 +3478,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="15"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="2" t="s">
         <v>88</v>
       </c>
@@ -3469,7 +3487,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="2" t="s">
         <v>88</v>
       </c>
@@ -3478,7 +3496,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="2" t="s">
         <v>88</v>
       </c>
@@ -3487,7 +3505,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="8" t="s">
         <v>89</v>
       </c>
@@ -3496,7 +3514,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="2" t="s">
         <v>89</v>
       </c>
@@ -3505,7 +3523,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="2" t="s">
         <v>89</v>
       </c>
@@ -3610,18 +3628,18 @@
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D56" s="1"/>
@@ -3630,18 +3648,18 @@
       <c r="G56" s="1"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3672,7 +3690,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -3686,7 +3704,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
+      <c r="A2" s="18"/>
       <c r="B2" s="2" t="s">
         <v>86</v>
       </c>
@@ -3698,7 +3716,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="2" t="s">
         <v>86</v>
       </c>
@@ -3710,7 +3728,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="2" t="s">
         <v>86</v>
       </c>
@@ -3722,7 +3740,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="2" t="s">
         <v>86</v>
       </c>
@@ -3734,7 +3752,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="8" t="s">
         <v>87</v>
       </c>
@@ -3746,7 +3764,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="2" t="s">
         <v>87</v>
       </c>
@@ -3758,7 +3776,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="2" t="s">
         <v>87</v>
       </c>
@@ -3770,7 +3788,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="8" t="s">
         <v>88</v>
       </c>
@@ -3782,7 +3800,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="2" t="s">
         <v>88</v>
       </c>
@@ -3794,7 +3812,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="2" t="s">
         <v>88</v>
       </c>
@@ -3806,7 +3824,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="2" t="s">
         <v>88</v>
       </c>
@@ -3818,7 +3836,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="2" t="s">
         <v>88</v>
       </c>
@@ -3830,7 +3848,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="2" t="s">
         <v>88</v>
       </c>
@@ -3842,7 +3860,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="2" t="s">
         <v>88</v>
       </c>
@@ -3854,7 +3872,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="8" t="s">
         <v>89</v>
       </c>
@@ -3866,7 +3884,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="2" t="s">
         <v>89</v>
       </c>
@@ -3878,7 +3896,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="2" t="s">
         <v>89</v>
       </c>

</xml_diff>